<commit_message>
Enhance summary generation in modern_torque_app; include MaxTorque with unit in summary data, update template structure, and improve placeholder handling for summary rows.
</commit_message>
<xml_diff>
--- a/summary_template.xlsx
+++ b/summary_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shop\Documents\Torque-Testing-App-V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCBDB0A-6AA3-4546-B067-A720E9816862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0B797E-0231-423B-A3B4-8DB825F5B73F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Manufacturer:</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Applied Torque</t>
   </si>
   <si>
-    <t>{{rows}}</t>
-  </si>
-  <si>
     <t>BURKE CALIBRATION LTD.</t>
   </si>
   <si>
@@ -147,6 +144,69 @@
   </si>
   <si>
     <t>{{CalibrationDue}}</t>
+  </si>
+  <si>
+    <t>{{AppliedTorque1}}</t>
+  </si>
+  <si>
+    <t>{{AppliedTorque2}}</t>
+  </si>
+  <si>
+    <t>{{AppliedTorque3}}</t>
+  </si>
+  <si>
+    <t>{{MinMaxAllowance1}}</t>
+  </si>
+  <si>
+    <t>{{MinMaxAllowance2}}</t>
+  </si>
+  <si>
+    <t>{{MinMaxAllowance3}}</t>
+  </si>
+  <si>
+    <t>{{Test1_Allowance1}}</t>
+  </si>
+  <si>
+    <t>{{Test1_Allowance2}}</t>
+  </si>
+  <si>
+    <t>{{Test1_Allowance3}}</t>
+  </si>
+  <si>
+    <t>{{Test2_Allowance1}}</t>
+  </si>
+  <si>
+    <t>{{Test2_Allowance2}}</t>
+  </si>
+  <si>
+    <t>{{Test2_Allowance3}}</t>
+  </si>
+  <si>
+    <t>{{Test3_Allowance1}}</t>
+  </si>
+  <si>
+    <t>{{Test3_Allowance2}}</t>
+  </si>
+  <si>
+    <t>{{Test3_Allowance3}}</t>
+  </si>
+  <si>
+    <t>{{Test4_Allowance1}}</t>
+  </si>
+  <si>
+    <t>{{Test4_Allowance2}}</t>
+  </si>
+  <si>
+    <t>{{Test4_Allowance3}}</t>
+  </si>
+  <si>
+    <t>{{Test5_Allowance1}}</t>
+  </si>
+  <si>
+    <t>{{Test5_Allowance2}}</t>
+  </si>
+  <si>
+    <t>{{Test5_Allowance3}}</t>
   </si>
 </sst>
 </file>
@@ -333,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -368,16 +428,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -394,7 +444,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -402,6 +451,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -450,28 +522,8 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -569,15 +621,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1021080</xdr:colOff>
+      <xdr:colOff>830580</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:rowOff>86360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>784860</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:rowOff>86360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -607,8 +659,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2179320" y="6682740"/>
-          <a:ext cx="891540" cy="541020"/>
+          <a:off x="1986280" y="7096760"/>
+          <a:ext cx="1122680" cy="584200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -917,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD581A7-1B59-4D68-AA4F-87BE84DB5952}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A14" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,7 +988,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -947,7 +999,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -958,7 +1010,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -978,7 +1030,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -989,7 +1041,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1003,15 +1055,15 @@
       <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
+      <c r="A8" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -1023,58 +1075,58 @@
       <c r="A10" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="39"/>
+      <c r="C10" s="25"/>
       <c r="E10" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="39" t="s">
+      <c r="F10" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="39"/>
+      <c r="G10" s="25"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="39"/>
+      <c r="C11" s="25"/>
       <c r="E11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="44"/>
+      <c r="F11" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="23"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="43"/>
+        <v>20</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="22"/>
       <c r="E12" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" s="44"/>
+      <c r="F12" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="23"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="39"/>
+      <c r="C13" s="25"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -1082,256 +1134,283 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
     </row>
     <row r="19" spans="1:7" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B19" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="36" t="s">
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+    </row>
+    <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A20" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" s="42" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A21" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A22" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" s="42" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="35" t="s">
+      <c r="B26" s="38"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="35"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="35"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="37" t="s">
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="40"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="40"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="40"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="40"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="40"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+    </row>
+    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="37"/>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="37"/>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="37"/>
-      <c r="B30" s="37"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="37"/>
-      <c r="B31" s="37"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="37"/>
-    </row>
-    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="17" t="s">
+      <c r="B33" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="35" t="s">
+      <c r="C33" s="38"/>
+    </row>
+    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="35"/>
-    </row>
-    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B34" s="38">
+      <c r="B34" s="41">
         <v>0.4</v>
       </c>
-      <c r="C34" s="38"/>
+      <c r="C34" s="41"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="26"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="28"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="31"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="29"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="31"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="34"/>
     </row>
     <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="35"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="37"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="16"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="B38" s="32"/>
-      <c r="C38" s="33"/>
-      <c r="D38" s="34"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="B41" s="35"/>
-      <c r="C41" s="35"/>
-      <c r="D41" s="35"/>
-      <c r="E41" s="35"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="35"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
     <mergeCell ref="B36:D38"/>
     <mergeCell ref="A41:G41"/>
     <mergeCell ref="C19:G19"/>
@@ -1340,8 +1419,22 @@
     <mergeCell ref="A27:G31"/>
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="F11:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup scale="84" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update .gitignore to prevent duplicate summary_template.xlsx entries and update summary_template.xlsx file.
</commit_message>
<xml_diff>
--- a/summary_template.xlsx
+++ b/summary_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shop\Documents\Torque-Testing-App-V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0B797E-0231-423B-A3B4-8DB825F5B73F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF106EE-2FC0-4BAB-84E8-A2999D9D4E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -286,7 +286,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -310,79 +310,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -393,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -434,13 +363,13 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -451,6 +380,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -461,69 +418,9 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -621,15 +518,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>830580</xdr:colOff>
+      <xdr:colOff>411480</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>86360</xdr:rowOff>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>784860</xdr:colOff>
+      <xdr:colOff>365760</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>86360</xdr:rowOff>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -659,7 +556,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1986280" y="7096760"/>
+          <a:off x="1567180" y="7566660"/>
           <a:ext cx="1122680" cy="584200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -970,7 +867,7 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A14" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1055,15 +952,15 @@
       <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -1075,58 +972,58 @@
       <c r="A10" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="25"/>
+      <c r="C10" s="27"/>
       <c r="E10" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="25"/>
+      <c r="G10" s="27"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="25"/>
+      <c r="C11" s="27"/>
       <c r="E11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="23"/>
+      <c r="G11" s="32"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="22"/>
+      <c r="C12" s="31"/>
       <c r="E12" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="F12" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="23"/>
+      <c r="G12" s="32"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="25"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -1136,46 +1033,46 @@
       <c r="A14" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
     </row>
     <row r="19" spans="1:7" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
@@ -1184,80 +1081,80 @@
       <c r="B19" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="39" t="s">
+      <c r="C19" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
     </row>
     <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="D20" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="42" t="s">
+      <c r="E20" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="42" t="s">
+      <c r="F20" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="42" t="s">
+      <c r="G20" s="22" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="42" t="s">
+      <c r="C21" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="D21" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="42" t="s">
+      <c r="E21" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="F21" s="42" t="s">
+      <c r="F21" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="42" t="s">
+      <c r="G21" s="22" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A22" s="42" t="s">
+      <c r="A22" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="42" t="s">
+      <c r="C22" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="42" t="s">
+      <c r="D22" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="42" t="s">
+      <c r="E22" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="42" t="s">
+      <c r="F22" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="G22" s="42" t="s">
+      <c r="G22" s="22" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1280,91 +1177,91 @@
       <c r="G24" s="21"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="38" t="s">
+      <c r="A25" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="38"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="38"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="40" t="s">
+      <c r="A27" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="40"/>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="40"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="40"/>
-      <c r="B28" s="40"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="40"/>
-      <c r="F28" s="40"/>
-      <c r="G28" s="40"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="40"/>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
+      <c r="A29" s="25"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="40"/>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
+      <c r="A30" s="25"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="40"/>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
     </row>
     <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="38" t="s">
+      <c r="B33" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="38"/>
+      <c r="C33" s="23"/>
     </row>
     <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="41">
+      <c r="B34" s="26">
         <v>0.4</v>
       </c>
-      <c r="C34" s="41"/>
+      <c r="C34" s="26"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
@@ -1372,22 +1269,22 @@
       <c r="C35" s="15"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="29"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="31"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="32"/>
-      <c r="C37" s="33"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
+    </row>
+    <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="34"/>
+      <c r="C37" s="34"/>
       <c r="D37" s="34"/>
     </row>
-    <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B38" s="35"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="37"/>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="34"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="16"/>
@@ -1399,19 +1296,31 @@
       <c r="G39" s="18"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="38" t="s">
+      <c r="A41" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B41" s="38"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="38"/>
-      <c r="F41" s="38"/>
-      <c r="G41" s="38"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="B36:D38"/>
+  <mergeCells count="20">
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
     <mergeCell ref="A41:G41"/>
     <mergeCell ref="C19:G19"/>
     <mergeCell ref="A25:G25"/>
@@ -1419,19 +1328,6 @@
     <mergeCell ref="A27:G31"/>
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="F11:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="84" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
``` Refactor summary generation logic in modern_torque_app for improved performance and maintainability ```
</commit_message>
<xml_diff>
--- a/summary_template.xlsx
+++ b/summary_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shop\Documents\Torque-Testing-App-V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF106EE-2FC0-4BAB-84E8-A2999D9D4E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59255B45-BA43-466C-A6C1-BCC096A62CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -383,17 +383,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -408,19 +410,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -450,7 +450,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>754380</xdr:colOff>
+      <xdr:colOff>1021080</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
@@ -524,7 +524,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>365760</xdr:colOff>
+      <xdr:colOff>480060</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
@@ -866,15 +866,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD581A7-1B59-4D68-AA4F-87BE84DB5952}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A14" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M41" sqref="M41"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="12.21875" style="3"/>
+    <col min="1" max="7" width="15.33203125" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="12.21875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -952,15 +951,15 @@
       <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -995,26 +994,26 @@
       <c r="E11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="32" t="s">
+      <c r="F11" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="32"/>
+      <c r="G11" s="25"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="31"/>
+      <c r="C12" s="24"/>
       <c r="E12" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="32" t="s">
+      <c r="F12" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="32"/>
+      <c r="G12" s="25"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
@@ -1081,13 +1080,13 @@
       <c r="B19" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
     </row>
     <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
@@ -1177,91 +1176,91 @@
       <c r="G24" s="21"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="25"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
+      <c r="A28" s="33"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
+      <c r="A29" s="33"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
+      <c r="A30" s="33"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="25"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
+      <c r="A31" s="33"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
     </row>
     <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="23" t="s">
+      <c r="B33" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="23"/>
+      <c r="C33" s="31"/>
     </row>
     <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="26">
+      <c r="B34" s="34">
         <v>0.4</v>
       </c>
-      <c r="C34" s="26"/>
+      <c r="C34" s="34"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
@@ -1269,22 +1268,22 @@
       <c r="C35" s="15"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="34"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="34"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
     </row>
     <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B37" s="34"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="34"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="34"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="34"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="16"/>
@@ -1296,18 +1295,31 @@
       <c r="G39" s="18"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="23" t="s">
+      <c r="A41" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B41" s="23"/>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23"/>
-      <c r="G41" s="23"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A41:G41"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A27:G31"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="A8:G8"/>
@@ -1315,19 +1327,6 @@
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="F11:G11"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="A41:G41"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A27:G31"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="84" orientation="portrait" r:id="rId1"/>

</xml_diff>